<commit_message>
[F/W] LEVEL LED - Power off시 같이 커지도록 수정
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/3_Firmware/Binary/Pipette SW Revision history.xlsx
+++ b/1_Plasma_Pipette/3_Firmware/Binary/Pipette SW Revision history.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +67,14 @@
   </si>
   <si>
     <t>GAS_EN 후 1.0sec 후 plasma On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level LED와 PWR LED 동기 시킴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -313,9 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,16 +330,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,6 +342,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -650,7 +658,7 @@
   <dimension ref="B4:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -662,119 +670,125 @@
   <sheetData>
     <row r="4" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:4" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="9">
+      <c r="B6" s="16">
         <v>43558</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="14">
+      <c r="B8" s="10">
         <v>43558</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="10">
+        <v>43565</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="13"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="13"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="13"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="14"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="13"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="13"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="14"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="14"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="13"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>

</xml_diff>

<commit_message>
4.1V Full charge 수정
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/3_Firmware/Binary/Pipette SW Revision history.xlsx
+++ b/1_Plasma_Pipette/3_Firmware/Binary/Pipette SW Revision history.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,30 @@
   </si>
   <si>
     <t>Level LED와 PWR LED 동기 시킴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\WORK\Project\3_Source\Test Sourse\V2.0_Source_20190403\plasma_pt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.10_1.0sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 1.0sec 후 plasma On, 4.1V 완충(ADC238)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.10_0.5sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 0.5sec 후 plasma On, 4.1V 완충(ADC238)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -307,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -342,6 +366,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D28"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -668,6 +701,14 @@
     <col min="4" max="4" width="57.125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="4" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:4" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
@@ -681,10 +722,10 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="16">
+      <c r="B6" s="19">
         <v>43558</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -692,8 +733,8 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
@@ -721,14 +762,26 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="10">
+        <v>43605</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="15">
+        <v>43605</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>

</xml_diff>

<commit_message>
Binary 정리하여 Femto에 release
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/3_Firmware/Binary/Pipette SW Revision history.xlsx
+++ b/1_Plasma_Pipette/3_Firmware/Binary/Pipette SW Revision history.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,55 +50,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>GAS_EN 후 0.5sec 후 plasma On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.00_0.5sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.00_1.0sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 1.0sec 후 plasma On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level LED와 PWR LED 동기 시킴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\WORK\Project\3_Source\Test Sourse\V2.0_Source_20190403\plasma_pt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.10_1.0sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 1.0sec 후 plasma On, 4.1V 완충(ADC238)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.10_0.5sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 0.5sec 후 plasma On, 4.1V 완충(ADC238)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.1_0.5sec_2,3,4msec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.1_1.0sec_2,3,4msec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.1_0.5sec_3,4,5msec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.1_1.0sec_3,4,5msec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Plasma On time 조정 : 30%, 40%, 50%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GAS_EN 후 0.5sec 후 plasma On</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V2.00_0.5sec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V2.00_1.0sec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GAS_EN 후 1.0sec 후 plasma On</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V2.01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Level LED와 PWR LED 동기 시킴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source Path</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\WORK\Project\3_Source\Test Sourse\V2.0_Source_20190403\plasma_pt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V2.10_1.0sec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GAS_EN 후 1.0sec 후 plasma On, 4.1V 완충(ADC238)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V2.10_0.5sec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GAS_EN 후 0.5sec 후 plasma On, 4.1V 완충(ADC238)</t>
+    <t>GAS_EN 후 0.5sec 후 plasma On, Plasma On time 조정 : 30%, 40%, 50%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 0.5sec 후 plasma On, Plasma On time 조정 : 20%, 30%, 40%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 1.0sec 후 plasma On, Plasma On time 조정 : 20%, 30%, 40%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS_EN 후 1.0sec 후 plasma On, Plasma On time 조정 : 30%, 40%, 50%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -139,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -327,11 +359,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,6 +454,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -691,22 +769,22 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.75" style="3" customWidth="1"/>
-    <col min="4" max="4" width="57.125" customWidth="1"/>
+    <col min="3" max="3" width="27.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -726,17 +804,17 @@
         <v>43558</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="20"/>
       <c r="C7" s="18"/>
       <c r="D7" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
@@ -744,10 +822,10 @@
         <v>43558</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
@@ -755,10 +833,10 @@
         <v>43565</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
@@ -766,10 +844,10 @@
         <v>43605</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -777,34 +855,52 @@
         <v>43605</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="9" t="s">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="21">
+        <v>43926</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="4"/>
       <c r="D16" s="9"/>
     </row>
@@ -859,9 +955,10 @@
       <c r="B28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B12:B16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>